<commit_message>
Add: Recursive Molecule Opening, Guessing System
</commit_message>
<xml_diff>
--- a/src/main/resources/database/default.xlsx
+++ b/src/main/resources/database/default.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craft\Documents\Projects\TCC\campo-quimico\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76064A27-FED8-450F-B78C-692D0733B526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80996B8-C678-4E00-84C4-B6CA5B0FD260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{29C8003B-5778-4769-A18F-77ACF920A148}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="29">
   <si>
     <t>H</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>SIMBOLO</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +606,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI23" sqref="AI23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,11 +649,11 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -720,31 +726,31 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -810,11 +816,11 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1680,7 +1686,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI23" sqref="AI23"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,11 +1729,11 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1800,31 +1806,31 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1890,11 +1896,11 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2759,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDB7A94-A861-4D02-9A53-730049F6237D}">
   <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AI23" sqref="AI23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add: Tips, Tip window, right click handler, molecule rotation
</commit_message>
<xml_diff>
--- a/src/main/resources/database/default.xlsx
+++ b/src/main/resources/database/default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craft\Documents\Projects\TCC\campo-quimico\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80996B8-C678-4E00-84C4-B6CA5B0FD260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D242030F-3151-4144-92E7-BC4886C0F581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{29C8003B-5778-4769-A18F-77ACF920A148}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{29C8003B-5778-4769-A18F-77ACF920A148}"/>
   </bookViews>
   <sheets>
     <sheet name="TESTE" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="45">
   <si>
     <t>H</t>
   </si>
@@ -125,6 +125,54 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>ELEMENTO A</t>
+  </si>
+  <si>
+    <t>ELEMENTO B</t>
+  </si>
+  <si>
+    <t>ELEMENTO C</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>ELEMENTO B 2</t>
+  </si>
+  <si>
+    <t>FAZ LIGAÇÃO TRIPLA</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ELEMENTO Y</t>
+  </si>
+  <si>
+    <t>ELEMENTO Z</t>
+  </si>
+  <si>
+    <t>ELEMENTO V1</t>
+  </si>
+  <si>
+    <t>ELEMENTO V2</t>
   </si>
 </sst>
 </file>
@@ -234,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -256,6 +304,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,7 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE765A9-04B5-4825-A496-2D36B425FA98}">
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,32 +668,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="Q1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="Q1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="12"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -707,13 +757,13 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>20</v>
@@ -732,19 +782,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>16</v>
@@ -759,13 +809,13 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>18</v>
@@ -795,20 +845,18 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
@@ -816,11 +864,11 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -833,16 +881,16 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>25</v>
@@ -1100,23 +1148,23 @@
       <c r="W17" s="1"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1686,7 +1734,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,42 +1746,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="Q1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="Q1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="12"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1787,13 +1835,13 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>20</v>
@@ -1806,31 +1854,31 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1839,13 +1887,13 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>18</v>
@@ -1875,13 +1923,13 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>19</v>
@@ -1896,16 +1944,16 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1913,13 +1961,13 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>18</v>
@@ -2180,23 +2228,23 @@
       <c r="W17" s="1"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -2765,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDB7A94-A861-4D02-9A53-730049F6237D}">
   <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI23" sqref="AI23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2778,32 +2826,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="Q1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="Q1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="12"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -3260,23 +3308,23 @@
       <c r="W17" s="1"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -3421,7 +3469,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
-      <c r="AI23" s="13"/>
+      <c r="AI23" s="9"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>

</xml_diff>